<commit_message>
BOM stuff for when we were building the board
</commit_message>
<xml_diff>
--- a/LRB_VikramProcter_V2.0.xlsx
+++ b/LRB_VikramProcter_V2.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\Documents\School\SOAR\LaunchRailBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8856F02C-E75D-4810-8CA5-D25F43E9EB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5707909-D00E-4D19-A88B-9789585482E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4A366B07-5FC2-40BD-B2E7-A05CA8CCFDAB}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="254">
   <si>
     <t>Name</t>
   </si>
@@ -792,6 +792,15 @@
   </si>
   <si>
     <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>KOA Speer Electronics, Inc.</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77796C1-099D-4B2D-87DC-F9839D30BED3}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1199,19 +1208,19 @@
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="26.44140625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="57.109375" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="26.44140625" customWidth="1"/>
-    <col min="13" max="13" width="23.109375" customWidth="1"/>
-    <col min="14" max="14" width="18.5546875" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+    <col min="4" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="114.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="14" max="14" width="20.109375" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1230,20 +1239,18 @@
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1262,20 +1269,18 @@
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1294,20 +1299,18 @@
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1326,20 +1329,18 @@
       <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="1"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1358,20 +1359,18 @@
       <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1390,20 +1389,18 @@
       <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="1"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1422,20 +1419,18 @@
       <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1454,20 +1449,18 @@
       <c r="F8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="1"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
@@ -1486,20 +1479,18 @@
       <c r="F9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -1518,18 +1509,18 @@
       <c r="F10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="L10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1548,20 +1539,18 @@
       <c r="F11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" s="1"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -1580,20 +1569,18 @@
       <c r="F12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -1612,20 +1599,18 @@
       <c r="F13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J13" s="1"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>72</v>
       </c>
@@ -1644,21 +1629,21 @@
       <c r="F14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" s="1"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>249</v>
       </c>
@@ -1674,18 +1659,18 @@
       <c r="F15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>80</v>
       </c>
@@ -1704,20 +1689,18 @@
       <c r="F16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>86</v>
       </c>
@@ -1736,20 +1719,18 @@
       <c r="F17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" s="1"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>91</v>
       </c>
@@ -1768,20 +1749,18 @@
       <c r="F18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>96</v>
       </c>
@@ -1800,21 +1779,21 @@
       <c r="F19" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J19" s="1"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="B20" s="2">
         <v>430450800</v>
       </c>
@@ -1830,18 +1809,18 @@
       <c r="F20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="1">
+        <v>430450800</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>104</v>
       </c>
@@ -1860,20 +1839,18 @@
       <c r="F21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J21" s="1"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>110</v>
       </c>
@@ -1892,20 +1869,18 @@
       <c r="F22" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J22" s="1"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>116</v>
       </c>
@@ -1924,20 +1899,18 @@
       <c r="F23" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="J23" s="1"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>122</v>
       </c>
@@ -1956,20 +1929,18 @@
       <c r="F24" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J24" s="1"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>127</v>
       </c>
@@ -1988,20 +1959,18 @@
       <c r="F25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J25" s="1"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -2020,20 +1989,18 @@
       <c r="F26" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J26" s="1"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
@@ -2052,20 +2019,18 @@
       <c r="F27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J27" s="1"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>143</v>
       </c>
@@ -2084,20 +2049,18 @@
       <c r="F28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J28" s="1"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>151</v>
       </c>
@@ -2116,20 +2079,18 @@
       <c r="F29" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J29" s="1"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>143</v>
       </c>
@@ -2148,20 +2109,18 @@
       <c r="F30" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J30" s="1"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -2180,20 +2139,18 @@
       <c r="F31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="J31" s="1"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
@@ -2212,20 +2169,18 @@
       <c r="F32" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J32" s="1"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
@@ -2244,20 +2199,18 @@
       <c r="F33" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J33" s="1"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>147</v>
       </c>
@@ -2276,20 +2229,18 @@
       <c r="F34" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="J34" s="1"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>181</v>
       </c>
@@ -2308,20 +2259,18 @@
       <c r="F35" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="J35" s="1"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>15</v>
       </c>
@@ -2340,20 +2289,18 @@
       <c r="F36" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="J36" s="1"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>190</v>
       </c>
@@ -2372,21 +2319,21 @@
       <c r="F37" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J37" s="1"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>252</v>
+      </c>
       <c r="B38" s="1" t="s">
         <v>145</v>
       </c>
@@ -2402,18 +2349,18 @@
       <c r="F38" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G38" s="2"/>
+      <c r="G38" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
       <c r="N38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>196</v>
       </c>
@@ -2432,20 +2379,18 @@
       <c r="F39" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="J39" s="1"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>202</v>
       </c>
@@ -2464,20 +2409,18 @@
       <c r="F40" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="J40" s="1"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>202</v>
       </c>
@@ -2496,21 +2439,21 @@
       <c r="F41" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>209</v>
+      </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="J41" s="1"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="B42" s="2" t="s">
         <v>210</v>
       </c>
@@ -2526,18 +2469,18 @@
       <c r="F42" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G42" s="2"/>
+      <c r="G42" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>80</v>
       </c>
@@ -2556,20 +2499,18 @@
       <c r="F43" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G43" s="2"/>
+      <c r="G43" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J43" s="1"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>220</v>
       </c>
@@ -2588,20 +2529,18 @@
       <c r="F44" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G44" s="2"/>
+      <c r="G44" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="J44" s="1"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>202</v>
       </c>
@@ -2620,20 +2559,18 @@
       <c r="F45" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G45" s="2"/>
+      <c r="G45" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="J45" s="1"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>231</v>
       </c>
@@ -2652,18 +2589,18 @@
       <c r="F46" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="G46" s="2"/>
+      <c r="G46" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
+      <c r="L46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O46" s="1"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>235</v>
       </c>
@@ -2682,20 +2619,18 @@
       <c r="F47" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G47" s="2"/>
+      <c r="G47" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J47" s="1"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>240</v>
       </c>
@@ -2714,20 +2649,18 @@
       <c r="F48" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="G48" s="2"/>
+      <c r="G48" s="2" t="s">
+        <v>242</v>
+      </c>
       <c r="H48" s="1"/>
-      <c r="I48" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="J48" s="1"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>246</v>
       </c>
@@ -2746,18 +2679,16 @@
       <c r="F49" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="G49" s="2"/>
+      <c r="G49" s="2" t="s">
+        <v>248</v>
+      </c>
       <c r="H49" s="1"/>
-      <c r="I49" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="J49" s="1"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>